<commit_message>
Updated Sprint Backlog and User Stories for Sprint 2.
</commit_message>
<xml_diff>
--- a/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
+++ b/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
   <si>
     <t>User story</t>
   </si>
@@ -194,6 +194,33 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>As a registrant I want to import atlethes from FriRes</t>
+  </si>
+  <si>
+    <t>As a registrant I want to import a startlist for a race from FriRes</t>
+  </si>
+  <si>
+    <t>As a registrant I want to import classes from FriRes</t>
+  </si>
+  <si>
+    <t>As a registrant I want to import races from FriRes</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>As a timekeeper I want to edit the timestamp list manually so I can correct errors during the race</t>
+  </si>
+  <si>
+    <t>As a registrant I want to edit the list with the order of the startnumbers at a checkpoint so I can correct errors during the race</t>
   </si>
 </sst>
 </file>
@@ -270,7 +297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -343,11 +370,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -412,12 +478,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -708,7 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1483,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1495,21 +1583,21 @@
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9" style="19" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21">
+    <row r="1" spans="1:8" ht="21">
       <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1">
       <c r="A3" s="17" t="s">
         <v>53</v>
       </c>
@@ -1522,18 +1610,22 @@
       <c r="D3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="27.75" thickBot="1">
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" ht="27.75" thickBot="1">
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7">
@@ -1542,17 +1634,19 @@
       <c r="D4" s="10">
         <v>3</v>
       </c>
-      <c r="E4" s="11">
-        <f t="shared" ref="E4:E32" si="0">D4/C4</f>
-        <v>3</v>
-      </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:7" ht="27.75" thickBot="1">
+      <c r="E4" s="21">
+        <f t="shared" ref="E4:E38" si="0">D4/C4</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="27.75" thickBot="1">
       <c r="A5" s="18">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="7">
@@ -1561,17 +1655,19 @@
       <c r="D5" s="10">
         <v>5</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="21">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" ht="27.75" thickBot="1">
+      <c r="F5" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="27.75" thickBot="1">
       <c r="A6" s="18">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7">
@@ -1580,17 +1676,19 @@
       <c r="D6" s="10">
         <v>5</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="21">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" ht="27.75" thickBot="1">
+      <c r="F6" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.75" thickBot="1">
       <c r="A7" s="18">
         <v>13</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7">
@@ -1599,17 +1697,19 @@
       <c r="D7" s="10">
         <v>5</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="21">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" ht="27.75" thickBot="1">
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="27.75" thickBot="1">
       <c r="A8" s="18">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="7">
@@ -1618,13 +1718,15 @@
       <c r="D8" s="10">
         <v>5</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="21">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" ht="27.75" thickBot="1">
+      <c r="F8" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="27.75" thickBot="1">
       <c r="A9" s="18">
         <v>15</v>
       </c>
@@ -1637,587 +1739,679 @@
       <c r="D9" s="10">
         <v>4</v>
       </c>
-      <c r="E9" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1">
+      <c r="E9" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1">
       <c r="A10" s="18">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7">
-        <v>3</v>
-      </c>
-      <c r="D10" s="10">
-        <v>5</v>
-      </c>
-      <c r="E10" s="11">
+        <v>56</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A11" s="18">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A12" s="18">
+        <v>37</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A13" s="18">
+        <v>38</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="1:8" ht="27.75" thickBot="1">
+      <c r="A14" s="18">
+        <v>39</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="27.75" thickBot="1">
+      <c r="A15" s="18">
+        <v>40</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A16" s="18">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="10">
+        <v>5</v>
+      </c>
+      <c r="E16" s="21">
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" ht="27.75" thickBot="1">
-      <c r="A11" s="18">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7">
-        <v>3</v>
-      </c>
-      <c r="D11" s="10">
-        <v>5</v>
-      </c>
-      <c r="E11" s="11">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:7" ht="27.75" thickBot="1">
-      <c r="A12" s="18">
-        <v>8</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7">
-        <v>3</v>
-      </c>
-      <c r="D12" s="10">
-        <v>5</v>
-      </c>
-      <c r="E12" s="11">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:7" ht="27.75" thickBot="1">
-      <c r="A13" s="18">
-        <v>21</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="7">
-        <v>3</v>
-      </c>
-      <c r="D13" s="10">
-        <v>5</v>
-      </c>
-      <c r="E13" s="11">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" ht="27.75" thickBot="1">
-      <c r="A14" s="18">
-        <v>12</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="7">
-        <v>2</v>
-      </c>
-      <c r="D14" s="10">
-        <v>3</v>
-      </c>
-      <c r="E14" s="11">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" ht="27.75" thickBot="1">
-      <c r="A15" s="18">
-        <v>25</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2</v>
-      </c>
-      <c r="D15" s="10">
-        <v>3</v>
-      </c>
-      <c r="E15" s="11">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A16" s="18">
-        <v>6</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="7">
-        <v>3</v>
-      </c>
-      <c r="D16" s="10">
-        <v>4</v>
-      </c>
-      <c r="E16" s="11">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="G16" s="14"/>
+      <c r="F16" s="23"/>
     </row>
     <row r="17" spans="1:7" ht="27.75" thickBot="1">
       <c r="A17" s="18">
-        <v>14</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="C17" s="7">
         <v>3</v>
       </c>
       <c r="D17" s="10">
-        <v>4</v>
-      </c>
-      <c r="E17" s="11">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" ht="41.25" thickBot="1">
+        <v>5</v>
+      </c>
+      <c r="E17" s="21">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F17" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="27.75" thickBot="1">
       <c r="A18" s="18">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C18" s="7">
         <v>3</v>
       </c>
       <c r="D18" s="10">
-        <v>4</v>
-      </c>
-      <c r="E18" s="11">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+        <v>5</v>
+      </c>
+      <c r="E18" s="21">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="1:7" ht="27.75" thickBot="1">
       <c r="A19" s="18">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C19" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D19" s="10">
         <v>5</v>
       </c>
-      <c r="E19" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G19" s="14"/>
+      <c r="E19" s="21">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F19" s="23"/>
     </row>
     <row r="20" spans="1:7" ht="27.75" thickBot="1">
       <c r="A20" s="18">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C20" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D20" s="10">
-        <v>5</v>
-      </c>
-      <c r="E20" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G20" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="E20" s="21">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="F20" s="23"/>
     </row>
     <row r="21" spans="1:7" ht="27.75" thickBot="1">
       <c r="A21" s="18">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C21" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="10">
         <v>3</v>
       </c>
-      <c r="E21" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" ht="27.75" thickBot="1">
+      <c r="E21" s="21">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="23"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1">
       <c r="A22" s="18">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C22" s="7">
         <v>3</v>
       </c>
       <c r="D22" s="10">
-        <v>3</v>
-      </c>
-      <c r="E22" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G22" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="E22" s="21">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:7" ht="27.75" thickBot="1">
       <c r="A23" s="18">
-        <v>28</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>49</v>
+        <v>14</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="7">
+        <v>3</v>
       </c>
       <c r="D23" s="10">
-        <v>5</v>
-      </c>
-      <c r="E23" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" spans="1:7" ht="27.75" thickBot="1">
+        <v>4</v>
+      </c>
+      <c r="E23" s="21">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="24" spans="1:7" ht="41.25" thickBot="1">
       <c r="A24" s="18">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C24" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="10">
-        <v>2</v>
-      </c>
-      <c r="E24" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" ht="27.75" thickBot="1">
+        <v>4</v>
+      </c>
+      <c r="E24" s="21">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F24" s="23"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1">
       <c r="A25" s="18">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C25" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25" s="10">
-        <v>3</v>
-      </c>
-      <c r="E25" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G25" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="E25" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F25" s="23"/>
     </row>
     <row r="26" spans="1:7" ht="27.75" thickBot="1">
       <c r="A26" s="18">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C26" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D26" s="10">
-        <v>2</v>
-      </c>
-      <c r="E26" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G26" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="E26" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:7" ht="27.75" thickBot="1">
       <c r="A27" s="18">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" s="10">
-        <v>1</v>
-      </c>
-      <c r="E27" s="11">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="F27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="E27" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F27" s="23"/>
     </row>
     <row r="28" spans="1:7" ht="27.75" thickBot="1">
       <c r="A28" s="18">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C28" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" s="10">
-        <v>1</v>
-      </c>
-      <c r="E28" s="11">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="F28" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7" ht="41.25" thickBot="1">
+        <v>3</v>
+      </c>
+      <c r="E28" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="1:7" ht="27.75" thickBot="1">
       <c r="A29" s="18">
-        <v>9</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="7">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="D29" s="10">
-        <v>2</v>
-      </c>
-      <c r="E29" s="11">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="G29" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="E29" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="23"/>
     </row>
     <row r="30" spans="1:7" ht="27.75" thickBot="1">
       <c r="A30" s="18">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C30" s="7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D30" s="10">
-        <v>3</v>
-      </c>
-      <c r="E30" s="11">
-        <f t="shared" si="0"/>
-        <v>0.375</v>
-      </c>
-      <c r="F30" t="s">
-        <v>51</v>
-      </c>
-      <c r="G30" s="14"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="27.75" thickBot="1">
       <c r="A31" s="18">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C31" s="7">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D31" s="10">
-        <v>4</v>
-      </c>
-      <c r="E31" s="11">
-        <f t="shared" si="0"/>
-        <v>0.30769230769230771</v>
-      </c>
-      <c r="G31" s="14"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1">
+        <v>3</v>
+      </c>
+      <c r="E31" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" spans="1:7" ht="27.75" thickBot="1">
       <c r="A32" s="18">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C32" s="7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D32" s="10">
-        <v>1</v>
-      </c>
-      <c r="E32" s="11">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-      <c r="G32" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="E32" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:7" ht="27.75" thickBot="1">
       <c r="A33" s="18">
-        <v>5</v>
-      </c>
-      <c r="B33" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="7">
+        <v>2</v>
+      </c>
+      <c r="D33" s="10">
+        <v>1</v>
+      </c>
+      <c r="E33" s="21">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F33" s="23"/>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="27.75" thickBot="1">
+      <c r="A34" s="18">
+        <v>31</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="7">
+        <v>2</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="21">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F34" s="23"/>
+      <c r="G34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="41.25" thickBot="1">
+      <c r="A35" s="18">
+        <v>9</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="7">
+        <v>5</v>
+      </c>
+      <c r="D35" s="10">
+        <v>2</v>
+      </c>
+      <c r="E35" s="21">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="F35" s="23"/>
+    </row>
+    <row r="36" spans="1:7" ht="27.75" thickBot="1">
+      <c r="A36" s="18">
+        <v>20</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="7">
+        <v>8</v>
+      </c>
+      <c r="D36" s="10">
+        <v>3</v>
+      </c>
+      <c r="E36" s="21">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="F36" s="23"/>
+      <c r="G36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A37" s="18">
+        <v>17</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="7">
+        <v>13</v>
+      </c>
+      <c r="D37" s="10">
+        <v>4</v>
+      </c>
+      <c r="E37" s="21">
+        <f t="shared" si="0"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="F37" s="23"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A38" s="18">
+        <v>18</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="7">
+        <v>8</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
+      <c r="E38" s="21">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="F38" s="23"/>
+    </row>
+    <row r="39" spans="1:7" ht="27.75" thickBot="1">
+      <c r="A39" s="18">
+        <v>5</v>
+      </c>
+      <c r="B39" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="10">
-        <v>2</v>
-      </c>
-      <c r="E33" s="11"/>
-      <c r="G33" s="14"/>
-    </row>
-    <row r="34" spans="1:7" ht="41.25" thickBot="1">
-      <c r="A34" s="18">
+      <c r="C39" s="15"/>
+      <c r="D39" s="10">
+        <v>2</v>
+      </c>
+      <c r="E39" s="21"/>
+      <c r="F39" s="23"/>
+    </row>
+    <row r="40" spans="1:7" ht="41.25" thickBot="1">
+      <c r="A40" s="18">
         <v>11</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B40" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="10">
-        <v>5</v>
-      </c>
-      <c r="E34" s="11"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" ht="27.75" thickBot="1">
-      <c r="A35" s="18">
+      <c r="C40" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="10">
+        <v>5</v>
+      </c>
+      <c r="E40" s="21"/>
+      <c r="F40" s="23"/>
+    </row>
+    <row r="41" spans="1:7" ht="27.75" thickBot="1">
+      <c r="A41" s="18">
         <v>19</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B41" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="10">
-        <v>2</v>
-      </c>
-      <c r="E35" s="11"/>
-      <c r="F35" t="s">
+      <c r="C41" s="15"/>
+      <c r="D41" s="10">
+        <v>2</v>
+      </c>
+      <c r="E41" s="21"/>
+      <c r="F41" s="23"/>
+      <c r="G41" t="s">
         <v>50</v>
       </c>
-      <c r="G35" s="14"/>
-    </row>
-    <row r="36" spans="1:7" ht="41.25" thickBot="1">
-      <c r="A36" s="18">
+    </row>
+    <row r="42" spans="1:7" ht="41.25" thickBot="1">
+      <c r="A42" s="18">
         <v>29</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B42" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="10">
-        <v>1</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" ht="27.75" thickBot="1">
-      <c r="A37" s="18">
+      <c r="C42" s="7"/>
+      <c r="D42" s="10">
+        <v>1</v>
+      </c>
+      <c r="E42" s="21"/>
+      <c r="F42" s="23"/>
+    </row>
+    <row r="43" spans="1:7" ht="27.75" thickBot="1">
+      <c r="A43" s="18">
         <v>34</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="7">
-        <v>3</v>
-      </c>
-      <c r="D37" s="10">
-        <v>5</v>
-      </c>
-      <c r="E37" s="11">
-        <f t="shared" ref="E37" si="1">D37/C37</f>
+      <c r="C43" s="7">
+        <v>3</v>
+      </c>
+      <c r="D43" s="10">
+        <v>5</v>
+      </c>
+      <c r="E43" s="21">
+        <f t="shared" ref="E43" si="1">D43/C43</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A38" s="16"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
-      <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A39" s="16"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
-      <c r="G39" s="14"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A40" s="16"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11"/>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A41" s="16"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
-      <c r="G41" s="14"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1"/>
+      <c r="F43" s="23"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A44" s="16"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="23"/>
+    </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1">
-      <c r="B45" s="8"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="23"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1">
-      <c r="B46" s="9"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="23"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1">
-      <c r="B47" s="5"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1">
-      <c r="B48" s="5"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="23"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" thickBot="1"/>
+    <row r="51" spans="2:2" ht="15.75" thickBot="1">
+      <c r="B51" s="8"/>
+    </row>
+    <row r="52" spans="2:2" ht="15.75" thickBot="1">
+      <c r="B52" s="9"/>
+    </row>
+    <row r="53" spans="2:2" ht="15.75" thickBot="1">
+      <c r="B53" s="5"/>
+    </row>
+    <row r="54" spans="2:2" ht="15.75" thickBot="1">
+      <c r="B54" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A4:G36">

</xml_diff>

<commit_message>
Updated Sprint Backlog with Sprint 4 and Backlog for the user stories.
</commit_message>
<xml_diff>
--- a/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
+++ b/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>User story</t>
   </si>
@@ -223,7 +223,19 @@
     <t>As a registrant I want to edit the list with the order of the startnumbers at a checkpoint so I can correct errors during the race</t>
   </si>
   <si>
-    <t>1, 2</t>
+    <t>As an Administrator I want to register checkpoints to a race</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Stories completed</t>
+  </si>
+  <si>
+    <t>Colors:</t>
+  </si>
+  <si>
+    <t>Stories in process</t>
   </si>
 </sst>
 </file>
@@ -292,12 +304,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -416,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -501,6 +525,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1579,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,19 +1632,26 @@
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="9" style="19" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>53</v>
       </c>
@@ -1628,12 +1674,15 @@
         <v>47</v>
       </c>
       <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7">
@@ -1643,18 +1692,18 @@
         <v>3</v>
       </c>
       <c r="E4" s="21">
-        <f t="shared" ref="E4:E40" si="0">D4/C4</f>
+        <f t="shared" ref="E4:E41" si="0">D4/C4</f>
         <v>3</v>
       </c>
       <c r="F4" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="7">
@@ -1671,11 +1720,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7">
@@ -1688,15 +1737,15 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F6" s="24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7">
@@ -1713,11 +1762,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="7">
@@ -1734,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>15</v>
       </c>
@@ -1753,11 +1802,11 @@
       </c>
       <c r="F9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>35</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="26" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1769,7 +1818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>36</v>
       </c>
@@ -1783,7 +1832,7 @@
       <c r="E11" s="21"/>
       <c r="F11" s="24"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>37</v>
       </c>
@@ -1797,7 +1846,7 @@
       <c r="E12" s="21"/>
       <c r="F12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>38</v>
       </c>
@@ -1811,11 +1860,11 @@
       <c r="E13" s="21"/>
       <c r="F13" s="24"/>
     </row>
-    <row r="14" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>39</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="27" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1827,11 +1876,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>40</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="27" t="s">
         <v>63</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1843,53 +1892,46 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
-        <v>1</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="7">
-        <v>3</v>
-      </c>
-      <c r="D16" s="10">
-        <v>5</v>
-      </c>
-      <c r="E16" s="21">
+        <v>41</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7">
+        <v>3</v>
+      </c>
+      <c r="D17" s="10">
+        <v>5</v>
+      </c>
+      <c r="E17" s="21">
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="F16" s="24"/>
-    </row>
-    <row r="17" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
-        <v>4</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="7">
-        <v>3</v>
-      </c>
-      <c r="D17" s="10">
-        <v>5</v>
-      </c>
-      <c r="E17" s="21">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>64</v>
-      </c>
+      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
+        <v>4</v>
+      </c>
+      <c r="B18" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C18" s="7">
         <v>3</v>
       </c>
@@ -1900,14 +1942,16 @@
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="24">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C19" s="7">
         <v>3</v>
@@ -1923,67 +1967,67 @@
     </row>
     <row r="20" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C20" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20" s="21">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
+        <v>12</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2</v>
+      </c>
+      <c r="D21" s="10">
+        <v>3</v>
+      </c>
+      <c r="E21" s="21">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18">
         <v>25</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="7">
-        <v>2</v>
-      </c>
-      <c r="D21" s="10">
-        <v>3</v>
-      </c>
-      <c r="E21" s="21">
+      <c r="C22" s="7">
+        <v>2</v>
+      </c>
+      <c r="D22" s="10">
+        <v>3</v>
+      </c>
+      <c r="E22" s="21">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="F21" s="24"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18">
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18">
         <v>6</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="26" t="s">
         <v>9</v>
-      </c>
-      <c r="C22" s="7">
-        <v>3</v>
-      </c>
-      <c r="D22" s="10">
-        <v>4</v>
-      </c>
-      <c r="E22" s="21">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18">
-        <v>14</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="C23" s="7">
         <v>3</v>
@@ -1995,14 +2039,16 @@
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="F23" s="24"/>
-    </row>
-    <row r="24" spans="1:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C24" s="7">
         <v>3</v>
@@ -2016,32 +2062,32 @@
       </c>
       <c r="F24" s="24"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
+        <v>26</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="7">
+        <v>3</v>
+      </c>
+      <c r="D25" s="10">
+        <v>4</v>
+      </c>
+      <c r="E25" s="21">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F25" s="24"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18">
         <v>7</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="7">
-        <v>5</v>
-      </c>
-      <c r="D25" s="10">
-        <v>5</v>
-      </c>
-      <c r="E25" s="21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F25" s="24"/>
-    </row>
-    <row r="26" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18">
-        <v>22</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="C26" s="7">
         <v>5</v>
       </c>
@@ -2052,20 +2098,22 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F26" s="24"/>
+      <c r="F26" s="24">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
+        <v>22</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="C27" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D27" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E27" s="21">
         <f t="shared" si="0"/>
@@ -2075,10 +2123,10 @@
     </row>
     <row r="28" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18">
+        <v>23</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="C28" s="7">
         <v>3</v>
@@ -2094,76 +2142,80 @@
     </row>
     <row r="29" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
-        <v>28</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>49</v>
+        <v>24</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="7">
+        <v>3</v>
       </c>
       <c r="D29" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E29" s="21">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F29" s="24"/>
+      <c r="F29" s="24">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18">
-        <v>30</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="7">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="D30" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E30" s="21">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F30" s="24"/>
-      <c r="G30" t="s">
-        <v>54</v>
+      <c r="F30" s="24">
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C31" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" s="21">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F31" s="24"/>
+      <c r="G31" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C32" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E32" s="21">
         <f t="shared" si="0"/>
@@ -2173,32 +2225,29 @@
     </row>
     <row r="33" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C33" s="7">
         <v>2</v>
       </c>
       <c r="D33" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="21">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F33" s="24"/>
-      <c r="G33" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="34" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C34" s="7">
         <v>2</v>
@@ -2212,180 +2261,194 @@
       </c>
       <c r="F34" s="24"/>
       <c r="G34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="18">
+        <v>31</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1</v>
+      </c>
+      <c r="E35" s="21">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F35" s="24"/>
+      <c r="G35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18">
+    <row r="36" spans="1:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18">
         <v>9</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="7">
-        <v>5</v>
-      </c>
-      <c r="D35" s="10">
-        <v>2</v>
-      </c>
-      <c r="E35" s="21">
+      <c r="C36" s="7">
+        <v>5</v>
+      </c>
+      <c r="D36" s="10">
+        <v>2</v>
+      </c>
+      <c r="E36" s="21">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="F35" s="24"/>
-    </row>
-    <row r="36" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18">
+      <c r="F36" s="24"/>
+    </row>
+    <row r="37" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="18">
         <v>20</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C37" s="7">
         <v>8</v>
       </c>
-      <c r="D36" s="10">
-        <v>3</v>
-      </c>
-      <c r="E36" s="21">
+      <c r="D37" s="10">
+        <v>3</v>
+      </c>
+      <c r="E37" s="21">
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
-      <c r="F36" s="24"/>
-      <c r="G36" t="s">
+      <c r="F37" s="24"/>
+      <c r="G37" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18">
-        <v>17</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="7">
-        <v>13</v>
-      </c>
-      <c r="D37" s="10">
-        <v>4</v>
-      </c>
-      <c r="E37" s="21">
-        <f t="shared" si="0"/>
-        <v>0.30769230769230771</v>
-      </c>
-      <c r="F37" s="24"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18">
+        <v>17</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="7">
+        <v>13</v>
+      </c>
+      <c r="D38" s="10">
+        <v>4</v>
+      </c>
+      <c r="E38" s="21">
+        <f t="shared" si="0"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="F38" s="24"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="18">
         <v>18</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C39" s="7">
         <v>8</v>
       </c>
-      <c r="D38" s="10">
-        <v>1</v>
-      </c>
-      <c r="E38" s="21">
+      <c r="D39" s="10">
+        <v>1</v>
+      </c>
+      <c r="E39" s="21">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="F38" s="24"/>
-    </row>
-    <row r="39" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18">
-        <v>5</v>
-      </c>
-      <c r="B39" s="12" t="s">
+      <c r="F39" s="24"/>
+    </row>
+    <row r="40" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18">
+        <v>5</v>
+      </c>
+      <c r="B40" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="10">
-        <v>2</v>
-      </c>
-      <c r="E39" s="21"/>
-      <c r="F39" s="24"/>
-    </row>
-    <row r="40" spans="1:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="18">
+      <c r="C40" s="15"/>
+      <c r="D40" s="10">
+        <v>2</v>
+      </c>
+      <c r="E40" s="21"/>
+      <c r="F40" s="24"/>
+    </row>
+    <row r="41" spans="1:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18">
         <v>11</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B41" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C41" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="10">
-        <v>5</v>
-      </c>
-      <c r="E40" s="21">
+      <c r="D41" s="10">
+        <v>5</v>
+      </c>
+      <c r="E41" s="21">
         <f t="shared" si="0"/>
         <v>0.625</v>
       </c>
-      <c r="F40" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18">
+      <c r="F41" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18">
         <v>19</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B42" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="10">
-        <v>2</v>
-      </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="24"/>
-      <c r="G41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="18">
-        <v>29</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="15"/>
       <c r="D42" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="21"/>
       <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
+        <v>29</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="10">
+        <v>1</v>
+      </c>
+      <c r="E43" s="21"/>
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18">
         <v>34</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="7">
-        <v>3</v>
-      </c>
-      <c r="D43" s="10">
-        <v>5</v>
-      </c>
-      <c r="E43" s="21">
-        <f t="shared" ref="E43" si="1">D43/C43</f>
+      <c r="C44" s="7">
+        <v>3</v>
+      </c>
+      <c r="D44" s="10">
+        <v>5</v>
+      </c>
+      <c r="E44" s="21">
+        <f t="shared" ref="E44" si="1">D44/C44</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="F43" s="24"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="23"/>
+      <c r="F44" s="24"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
@@ -2411,22 +2474,30 @@
       <c r="E47" s="21"/>
       <c r="F47" s="23"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="50" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="8"/>
-    </row>
-    <row r="52" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="9"/>
-    </row>
-    <row r="53" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="5"/>
-    </row>
-    <row r="54" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="16"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="23"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="51" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="8"/>
+    </row>
+    <row r="53" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="9"/>
+    </row>
+    <row r="54" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="5"/>
+    </row>
+    <row r="55" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A4:G36">

</xml_diff>

<commit_message>
Refactor tests added club
</commit_message>
<xml_diff>
--- a/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
+++ b/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="14880" windowHeight="7605" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="14640" windowHeight="7335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories (Not updated)" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
   <si>
     <t>User story</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>As a registrant I want to print the result list so that I can distribute the results physically.</t>
+  </si>
+  <si>
+    <t>As an administrator I want to tie races to an event so that I can group the races by events.</t>
   </si>
 </sst>
 </file>
@@ -1706,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1741,7 +1744,7 @@
       <c r="A3" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1982,7 +1985,7 @@
       <c r="A16" s="18">
         <v>41</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="26" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -1996,7 +1999,7 @@
       <c r="A17" s="18">
         <v>1</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="7">
@@ -2036,7 +2039,7 @@
       <c r="A19" s="18">
         <v>8</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="7">
@@ -2093,7 +2096,7 @@
       <c r="A22" s="18">
         <v>25</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="7">
@@ -2112,7 +2115,7 @@
       <c r="A23" s="18">
         <v>6</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="7">
@@ -2171,7 +2174,7 @@
       <c r="A26" s="18">
         <v>7</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="7">
@@ -2251,7 +2254,7 @@
       <c r="A30" s="18">
         <v>28</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="15" t="s">
@@ -2313,7 +2316,7 @@
       <c r="A33" s="18">
         <v>33</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="26" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="7">
@@ -2512,7 +2515,7 @@
       <c r="A43" s="18">
         <v>29</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="26" t="s">
         <v>72</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -2606,7 +2609,7 @@
       <c r="A49" s="16">
         <v>46</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="26" t="s">
         <v>75</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -2616,9 +2619,20 @@
       <c r="E49" s="21"/>
       <c r="F49" s="23"/>
     </row>
-    <row r="50" spans="1:6" ht="15.75" thickBot="1">
-      <c r="B50" s="5"/>
-      <c r="C50" s="2"/>
+    <row r="50" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A50" s="16">
+        <f>MAX(A4:A49)+1</f>
+        <v>47</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="10"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="23"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1">
       <c r="B51" s="5"/>

</xml_diff>

<commit_message>
Delete database updated timers
</commit_message>
<xml_diff>
--- a/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
+++ b/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
@@ -1705,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2489,7 +2489,7 @@
       <c r="A42" s="18">
         <v>19</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="30" t="s">
         <v>44</v>
       </c>
       <c r="C42" s="15" t="s">

</xml_diff>

<commit_message>
made changes to the timer and menu structure and fixing bugs
</commit_message>
<xml_diff>
--- a/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
+++ b/doc/Backlogs/ITimeU_User_stories_estimated.xlsx
@@ -523,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -607,10 +607,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1705,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1725,14 +1721,14 @@
         <v>42</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="28" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1740,7 +1736,7 @@
       <c r="A3" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1759,7 +1755,7 @@
         <v>47</v>
       </c>
       <c r="H3" s="13"/>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="26" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1767,7 +1763,7 @@
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7">
@@ -1788,7 +1784,7 @@
       <c r="A5" s="18">
         <v>2</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="7">
@@ -1809,7 +1805,7 @@
       <c r="A6" s="18">
         <v>10</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7">
@@ -1830,7 +1826,7 @@
       <c r="A7" s="18">
         <v>13</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7">
@@ -1851,7 +1847,7 @@
       <c r="A8" s="18">
         <v>16</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="7">
@@ -1891,7 +1887,7 @@
       <c r="A10" s="18">
         <v>35</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1949,7 +1945,7 @@
       <c r="A14" s="18">
         <v>39</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1965,7 +1961,7 @@
       <c r="A15" s="18">
         <v>40</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>63</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1981,7 +1977,7 @@
       <c r="A16" s="18">
         <v>41</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -1995,7 +1991,7 @@
       <c r="A17" s="18">
         <v>1</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="7">
@@ -2014,7 +2010,7 @@
       <c r="A18" s="18">
         <v>4</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="7">
@@ -2035,7 +2031,7 @@
       <c r="A19" s="18">
         <v>8</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="7">
@@ -2092,7 +2088,7 @@
       <c r="A22" s="18">
         <v>25</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="7">
@@ -2111,7 +2107,7 @@
       <c r="A23" s="18">
         <v>6</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="7">
@@ -2132,7 +2128,7 @@
       <c r="A24" s="18">
         <v>14</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="7">
@@ -2170,7 +2166,7 @@
       <c r="A26" s="18">
         <v>7</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="7">
@@ -2191,7 +2187,7 @@
       <c r="A27" s="18">
         <v>22</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="7">
@@ -2250,7 +2246,7 @@
       <c r="A30" s="18">
         <v>28</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C30" s="15" t="s">
@@ -2312,7 +2308,7 @@
       <c r="A33" s="18">
         <v>33</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="7">
@@ -2394,7 +2390,7 @@
       <c r="A37" s="18">
         <v>20</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="25" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="7">
@@ -2454,7 +2450,7 @@
       <c r="A40" s="18">
         <v>5</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="29" t="s">
         <v>40</v>
       </c>
       <c r="C40" s="15"/>
@@ -2468,7 +2464,7 @@
       <c r="A41" s="18">
         <v>11</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="30" t="s">
         <v>41</v>
       </c>
       <c r="C41" s="15" t="s">
@@ -2489,7 +2485,7 @@
       <c r="A42" s="18">
         <v>19</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="25" t="s">
         <v>44</v>
       </c>
       <c r="C42" s="15" t="s">
@@ -2511,7 +2507,7 @@
       <c r="A43" s="18">
         <v>29</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="25" t="s">
         <v>72</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -2530,7 +2526,7 @@
       <c r="A44" s="18">
         <v>34</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="29" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="7">
@@ -2605,7 +2601,7 @@
       <c r="A49" s="16">
         <v>46</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="25" t="s">
         <v>75</v>
       </c>
       <c r="C49" s="7" t="s">

</xml_diff>